<commit_message>
small revisions, add demonstration file
</commit_message>
<xml_diff>
--- a/csv_format_standard_20200825.xlsx
+++ b/csv_format_standard_20200825.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qnw/Dropbox (ORNL)/ESS-DIVE/csv/2standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028FCFB8-D1F1-7948-8E90-296488DABAB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7B23DE-54C3-5C43-80C9-17F233AB2320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="10720" xr2:uid="{23270E26-11E1-EE40-BC5A-96F6ED97C00E}"/>
   </bookViews>
@@ -174,30 +174,6 @@
   </si>
   <si>
     <r>
-      <t>All dates and times must be reported in Coordinated Universal Time (UTC) and follow the ISO 8601 standard (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RFC 3339</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>). All times must be preceded with a date. In cases where the entire file consists of temporal data collected at a single date and time, the date and time must be documented elsewhere if not provided as a variable. Temporal data using different standards can be provided as a separate variable (i.e., in an adjacent column) in addition to UTC format.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>All geographic coordinates must be provided in WGS84 decimal format (</t>
     </r>
     <r>
@@ -320,6 +296,30 @@
   </si>
   <si>
     <t>Use unique, descriptive variable names.</t>
+  </si>
+  <si>
+    <r>
+      <t>All dates and times must be reported in Coordinated Universal Time (UTC) and follow the ISO 8601 standard (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RFC 3339</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>). Note that the use of "Z" and "T" characters are unnecessary. All times must be preceded with a date. In cases where the entire file consists of temporal data collected at a single date and time, the date and time must be documented elsewhere if not provided as a variable. Temporal data using different standards can be provided as a separate variable (i.e., in an adjacent column) in addition to UTC format.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE8B38F-3DD4-AA4C-8221-71A87F25D7F3}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -910,7 +910,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
@@ -975,10 +975,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
@@ -995,7 +995,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>5</v>
@@ -1052,7 +1052,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="85">
+    <row r="18" spans="1:5" ht="102">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
@@ -1097,7 +1097,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
@@ -1110,27 +1110,27 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small updates, added crosswalk
</commit_message>
<xml_diff>
--- a/csv_format_standard_20200825.xlsx
+++ b/csv_format_standard_20200825.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qnw/Dropbox (ORNL)/ESS-DIVE/csv/2standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7B23DE-54C3-5C43-80C9-17F233AB2320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74436D5-C2B0-A94B-8E47-A8D86860E2A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="10720" xr2:uid="{23270E26-11E1-EE40-BC5A-96F6ED97C00E}"/>
+    <workbookView xWindow="8940" yWindow="2600" windowWidth="19860" windowHeight="15400" xr2:uid="{23270E26-11E1-EE40-BC5A-96F6ED97C00E}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="1" r:id="rId1"/>
@@ -149,9 +149,6 @@
     <t>If a cell does not contain a value, a missing data value must be indicated. Missing data must be represented by values that can never be construed as actual data and must be consistent across variables. For columns containing numeric data, "-9999" is preferred as the missing data value or use the correct precision given the data in the column. For columns containing character data, the string "NA" is preferred as the missing data value. Explanations for individual missing values can be reported as a separate variable (i.e., in an adjacent column). If a coding system is used to describe the missing data value, it must be documented elsewhere.</t>
   </si>
   <si>
-    <t>Measurement uncertainty, limits of detection, data quality indicators, and other flags pertaining to individual values should be reported as a separate variable (i.e., in an adjacent column). If a coding system is used to describe the flags, it must be documented elsewhere.</t>
-  </si>
-  <si>
     <t>Provide temporal data in UTC format.</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>Provide spatial data in WGS84 decimal format.</t>
   </si>
   <si>
-    <t>For timestamped data, the variable name should specify if the measurement is the start, stop, or midpoint value, or it must be documented elsewhere.</t>
-  </si>
-  <si>
     <t>Provide variable measurement uncertainty, limits of detection, data quality indicators, and other flags.</t>
   </si>
   <si>
@@ -171,30 +165,6 @@
   </si>
   <si>
     <t>References are shown in bold and sources are listed at the bottom of the table.</t>
-  </si>
-  <si>
-    <r>
-      <t>All geographic coordinates must be provided in WGS84 decimal format (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EPSG 4326</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>). Latitude and longitude must be provided as separate variables (i.e., in an adjacent column). In cases where the entire file consists of measurements collected at a single location, a pair of geographic coordinates must be documented elsewhere if not provided as a variable. Spatial data using different standards can be provided as a separate variable (i.e., in an adjacent column) in addition to WGS84 decimal format.</t>
-    </r>
   </si>
   <si>
     <t>RFC 4180, https://tools.ietf.org/html/rfc4180</t>
@@ -260,18 +230,6 @@
   </si>
   <si>
     <r>
-      <t>Unique variable names must be us</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>ed. No spaces.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Provide the units of measurement for the variable in the variable name following the same naming conventions for the variable (e.g., total_depth_cm)). If units are not provided here, it must be documented elsewhere. Data should be represented with units of measurement approved by the International System of Units (</t>
     </r>
     <r>
@@ -299,6 +257,33 @@
   </si>
   <si>
     <r>
+      <t>All geographic coordinates must be provided in WGS84 decimal format (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EPSG 4326</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>). Latitude and longitude must be provided as separate variables (i.e., in an adjacent column). For geolocated records, each row must contain coordinates. In cases where the entire file consists of measurements collected at a single location, a pair of geographic coordinates must be documented elsewhere if not provided as variables. Spatial data using different standards can be provided as a separate variable (i.e., in an adjacent column) but only in addition to WGS84 decimal format.</t>
+    </r>
+  </si>
+  <si>
+    <t>For data with multiple timestamped records or when applicable, the variable name should specify if the measurement is the start, stop, or midpoint value, or it shoild be documented elsewhere.</t>
+  </si>
+  <si>
+    <r>
       <t>All dates and times must be reported in Coordinated Universal Time (UTC) and follow the ISO 8601 standard (</t>
     </r>
     <r>
@@ -318,7 +303,31 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>). Note that the use of "Z" and "T" characters are unnecessary. All times must be preceded with a date. In cases where the entire file consists of temporal data collected at a single date and time, the date and time must be documented elsewhere if not provided as a variable. Temporal data using different standards can be provided as a separate variable (i.e., in an adjacent column) in addition to UTC format.</t>
+      <t>). Note that the use of "Z" and "T" characters are unnecessary. All times must be preceded with a date. In cases where the entire file consists of temporal data collected at a single date and time, the date and time must be documented elsewhere if not provided as a variable. Temporal data using different standards can be provided as a separate variable (i.e., in an adjacent column) but only in addition to UTC format.</t>
+    </r>
+  </si>
+  <si>
+    <t>Measurement uncertainty, limits of detection, data quality indicators, and other flags pertaining to individual values should be reported as a separate variable (i.e., in an adjacent column) but only in addition to the reported values. If a coding system is used to describe the flags, it must be documented elsewhere.</t>
+  </si>
+  <si>
+    <r>
+      <t>Unique variable names must be us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>ed. No spaces.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Letters, numbers, a hyphen "-" (ASCII Code 45), and an underscore "_" (ASCII Code 95) are preferred in variable names.</t>
     </r>
   </si>
 </sst>
@@ -838,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAE8B38F-3DD4-AA4C-8221-71A87F25D7F3}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -879,7 +888,7 @@
     </row>
     <row r="6" spans="1:5" ht="19">
       <c r="A6" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19">
@@ -910,7 +919,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>5</v>
@@ -967,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17">
+    <row r="13" spans="1:5" ht="34">
       <c r="A13" s="8" t="s">
         <v>14</v>
       </c>
@@ -975,10 +984,10 @@
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>5</v>
@@ -995,7 +1004,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>5</v>
@@ -1035,7 +1044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="51">
+    <row r="17" spans="1:5" ht="68">
       <c r="A17" s="8" t="s">
         <v>18</v>
       </c>
@@ -1043,10 +1052,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>6</v>
@@ -1060,16 +1069,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="34">
+    <row r="19" spans="1:5" ht="51">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -1077,16 +1086,16 @@
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="102">
+    <row r="20" spans="1:5" ht="119">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -1094,10 +1103,10 @@
         <v>9</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>5</v>
@@ -1105,32 +1114,32 @@
     </row>
     <row r="21" spans="1:5" ht="19">
       <c r="A21" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>